<commit_message>
inserted results from test 9.1
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 0.xlsx
+++ b/Data Collections/Data Collection Sim 0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umeer\Desktop\University\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CEAE53-E0A2-4D1E-A631-5F58A5FB2A77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABFCFD-3EDA-48FD-8399-0596D0A78595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -344,13 +344,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0.000000000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
     <numFmt numFmtId="167" formatCode="0.00000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -609,7 +608,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,7 +672,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -687,10 +685,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -17753,8 +17751,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5553074" y="595312"/>
-              <a:ext cx="4733925" cy="2867025"/>
+              <a:off x="5554979" y="591502"/>
+              <a:ext cx="4732020" cy="2842260"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -17867,8 +17865,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5667375" y="12277725"/>
-              <a:ext cx="4733925" cy="2733675"/>
+              <a:off x="5669280" y="12184380"/>
+              <a:ext cx="4732020" cy="2735580"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -18722,7 +18720,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -18766,7 +18764,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -18808,7 +18806,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -18854,7 +18852,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -18897,7 +18895,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -18943,7 +18941,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -18989,7 +18987,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -19035,7 +19033,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="5">
@@ -19083,7 +19081,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -19129,7 +19127,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -19175,7 +19173,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -19219,7 +19217,7 @@
       <c r="T12" s="23"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="39" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6">
@@ -19264,7 +19262,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -19307,7 +19305,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -19350,7 +19348,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -19393,7 +19391,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -19436,7 +19434,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -19524,7 +19522,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="30">
@@ -19573,7 +19571,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="30">
         <v>2</v>
       </c>
@@ -19620,7 +19618,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="37" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="10">
@@ -19665,7 +19663,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -19708,7 +19706,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -19751,7 +19749,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -19794,7 +19792,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -19837,7 +19835,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="12">
@@ -19885,7 +19883,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -19928,7 +19926,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -19971,7 +19969,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -20014,7 +20012,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -20057,7 +20055,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -20100,7 +20098,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="14">
@@ -20145,7 +20143,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -20188,7 +20186,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -20231,7 +20229,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -20274,7 +20272,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -20317,7 +20315,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="37" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="20">
@@ -20358,7 +20356,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="20">
         <v>2</v>
       </c>
@@ -20397,7 +20395,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="20">
         <v>3</v>
       </c>
@@ -20436,7 +20434,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="20">
         <v>4</v>
       </c>
@@ -20475,7 +20473,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="20">
         <v>5</v>
       </c>
@@ -20514,7 +20512,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="37" t="s">
         <v>93</v>
       </c>
       <c r="B43" s="24">
@@ -20558,7 +20556,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="24">
         <v>2</v>
       </c>
@@ -20600,7 +20598,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="24">
         <v>3</v>
       </c>
@@ -20642,7 +20640,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="24">
         <v>4</v>
       </c>
@@ -20684,7 +20682,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="38"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="24">
         <v>5</v>
       </c>
@@ -20726,7 +20724,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="24">
         <v>6</v>
       </c>
@@ -21697,18 +21695,18 @@
       <c r="J41" t="s">
         <v>90</v>
       </c>
-      <c r="K41" s="43" t="s">
+      <c r="K41" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43" t="s">
+      <c r="L41" s="41"/>
+      <c r="M41" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43" t="s">
+      <c r="N41" s="41"/>
+      <c r="O41" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="P41" s="43"/>
+      <c r="P41" s="41"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -21735,18 +21733,18 @@
       <c r="J42">
         <v>10</v>
       </c>
-      <c r="K42" s="43">
+      <c r="K42" s="41">
         <v>1.2</v>
       </c>
-      <c r="L42" s="43"/>
-      <c r="M42" s="43">
+      <c r="L42" s="41"/>
+      <c r="M42" s="41">
         <v>3</v>
       </c>
-      <c r="N42" s="43"/>
-      <c r="O42" s="43">
+      <c r="N42" s="41"/>
+      <c r="O42" s="41">
         <v>1.7929999999999999</v>
       </c>
-      <c r="P42" s="43"/>
+      <c r="P42" s="41"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -21773,18 +21771,18 @@
       <c r="J43">
         <v>20</v>
       </c>
-      <c r="K43" s="43">
+      <c r="K43" s="41">
         <v>1.3</v>
       </c>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43">
+      <c r="L43" s="41"/>
+      <c r="M43" s="41">
         <v>4</v>
       </c>
-      <c r="N43" s="43"/>
-      <c r="O43" s="43">
+      <c r="N43" s="41"/>
+      <c r="O43" s="41">
         <v>1.8839999999999999</v>
       </c>
-      <c r="P43" s="43"/>
+      <c r="P43" s="41"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -21811,18 +21809,18 @@
       <c r="J44">
         <v>50</v>
       </c>
-      <c r="K44" s="43">
+      <c r="K44" s="41">
         <v>2.36</v>
       </c>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43">
+      <c r="L44" s="41"/>
+      <c r="M44" s="41">
         <v>6</v>
       </c>
-      <c r="N44" s="43"/>
-      <c r="O44" s="43">
+      <c r="N44" s="41"/>
+      <c r="O44" s="41">
         <v>2.2669999999999999</v>
       </c>
-      <c r="P44" s="43"/>
+      <c r="P44" s="41"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -21849,18 +21847,18 @@
       <c r="J45">
         <v>100</v>
       </c>
-      <c r="K45" s="43">
+      <c r="K45" s="41">
         <v>2.5499999999999998</v>
       </c>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43">
+      <c r="L45" s="41"/>
+      <c r="M45" s="41">
         <v>8</v>
       </c>
-      <c r="N45" s="43"/>
-      <c r="O45" s="43">
+      <c r="N45" s="41"/>
+      <c r="O45" s="41">
         <v>2.8820000000000001</v>
       </c>
-      <c r="P45" s="43"/>
+      <c r="P45" s="41"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -21887,12 +21885,12 @@
       <c r="J46">
         <v>500</v>
       </c>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43"/>
-      <c r="P46" s="43"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="41"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -21919,18 +21917,18 @@
       <c r="J47">
         <v>1000</v>
       </c>
-      <c r="K47" s="43">
+      <c r="K47" s="41">
         <v>3.55</v>
       </c>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43">
+      <c r="L47" s="41"/>
+      <c r="M47" s="41">
         <v>12</v>
       </c>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43">
+      <c r="N47" s="41"/>
+      <c r="O47" s="41">
         <v>4.1079999999999997</v>
       </c>
-      <c r="P47" s="43"/>
+      <c r="P47" s="41"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48">
@@ -23040,6 +23038,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J40:P40"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
     <mergeCell ref="O47:P47"/>
     <mergeCell ref="K47:L47"/>
     <mergeCell ref="M43:N43"/>
@@ -23052,16 +23060,6 @@
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="O46:P46"/>
-    <mergeCell ref="J40:P40"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23072,7 +23070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8ADDF3-F6DC-49DE-90F6-6F07047D1F12}">
   <dimension ref="A1:Q1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -47323,19 +47321,19 @@
       <c r="G103" s="28"/>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="44"/>
+      <c r="A108" s="43"/>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="44"/>
+      <c r="A109" s="43"/>
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="44"/>
+      <c r="A110" s="43"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="44"/>
+      <c r="A111" s="43"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -49227,14 +49225,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE4954-B822-463F-AF49-CD5C62D3DBE0}">
   <dimension ref="A1:AA105"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -49263,7 +49261,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="37">
+      <c r="B2" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C2" s="33">
@@ -49280,7 +49278,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="37">
+      <c r="B3" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C3" s="33">
@@ -49297,8 +49295,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="37">
-        <v>0.406666666668</v>
+      <c r="B4" s="33">
+        <v>44.855114553641997</v>
       </c>
       <c r="C4" s="33">
         <v>0.50833333333499997</v>
@@ -49314,7 +49312,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="37">
+      <c r="B5" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C5" s="33">
@@ -49331,8 +49329,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="37">
-        <v>0.406666666668</v>
+      <c r="B6" s="33">
+        <v>181.92077979172399</v>
       </c>
       <c r="C6" s="33">
         <v>0.50833333333499997</v>
@@ -49348,7 +49346,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="37">
+      <c r="B7" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C7" s="33">
@@ -49365,7 +49363,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="37">
+      <c r="B8" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C8" s="33">
@@ -49382,7 +49380,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
+      <c r="B9" s="33">
         <v>0.406666666668</v>
       </c>
       <c r="C9" s="33">
@@ -49399,7 +49397,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C10" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49414,7 +49414,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+      <c r="B11" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C11" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49429,7 +49431,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
+      <c r="B12" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C12" s="33">
         <v>0.406666666668</v>
       </c>
@@ -49444,7 +49448,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
+      <c r="B13" s="33">
+        <v>0.30500000000100003</v>
+      </c>
       <c r="C13" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49459,7 +49465,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
+      <c r="B14" s="33">
+        <v>36.394076976145001</v>
+      </c>
       <c r="C14" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49474,7 +49482,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
+      <c r="B15" s="33">
+        <v>22.100444436389001</v>
+      </c>
       <c r="C15" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49489,7 +49499,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
+      <c r="B16" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C16" s="33">
         <v>95.678212007157001</v>
       </c>
@@ -49504,7 +49516,9 @@
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
+      <c r="B17" s="33">
+        <v>41.417893529856997</v>
+      </c>
       <c r="C17" s="33">
         <v>75.810779305322995</v>
       </c>
@@ -49519,7 +49533,9 @@
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
+      <c r="B18" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C18" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49534,7 +49550,9 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
+      <c r="B19" s="33">
+        <v>32.247614029048997</v>
+      </c>
       <c r="C19" s="33">
         <v>156.30260621395999</v>
       </c>
@@ -49549,7 +49567,9 @@
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
+      <c r="B20" s="33">
+        <v>53.063883783317003</v>
+      </c>
       <c r="C20" s="33">
         <v>0.406666666668</v>
       </c>
@@ -49564,7 +49584,9 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
+      <c r="B21" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C21" s="33">
         <v>0.50833333333499997</v>
       </c>
@@ -49579,7 +49601,9 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
+      <c r="B22" s="33">
+        <v>0.406666666668</v>
+      </c>
       <c r="C22" s="33">
         <v>0.50833333333499997</v>
       </c>

</xml_diff>

<commit_message>
inserted results form q6.4 and t8.2
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 0.xlsx
+++ b/Data Collections/Data Collection Sim 0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E1E94-21FE-428A-AC21-D84FC624CCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0845A7F5-DB18-4663-B97A-43B5FA032FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="3024" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="4656" yWindow="1776" windowWidth="17280" windowHeight="9024" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="Set9" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -662,6 +662,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -675,13 +676,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="60% - Accent1" xfId="10" builtinId="32"/>
@@ -2960,7 +2960,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2998,7 +2998,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -3026,7 +3026,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3064,7 +3064,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -7055,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -7132,7 +7132,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="4">
@@ -7176,7 +7176,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -7218,7 +7218,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -7262,7 +7262,7 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -7305,7 +7305,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -7393,7 +7393,7 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -7437,7 +7437,7 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="47" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5">
@@ -7483,7 +7483,7 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -7527,7 +7527,7 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -7571,7 +7571,7 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -7615,7 +7615,7 @@
       <c r="T12" s="22"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="47" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="6">
@@ -7660,7 +7660,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -7703,7 +7703,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -7746,7 +7746,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -7789,7 +7789,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -7832,7 +7832,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -7920,7 +7920,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="29">
@@ -7969,7 +7969,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="29">
         <v>2</v>
       </c>
@@ -8016,7 +8016,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="10">
@@ -8061,7 +8061,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="44"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -8104,7 +8104,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="44"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -8147,7 +8147,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -8190,7 +8190,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -8233,7 +8233,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="45" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="12">
@@ -8281,7 +8281,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="44"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -8324,7 +8324,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="44"/>
+      <c r="A29" s="45"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -8367,7 +8367,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="44"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -8410,7 +8410,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="44"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -8453,7 +8453,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="44"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -8496,7 +8496,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="14">
@@ -8541,7 +8541,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -8584,7 +8584,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="44"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -8627,7 +8627,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="44"/>
+      <c r="A36" s="45"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -8713,7 +8713,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="45" t="s">
         <v>85</v>
       </c>
       <c r="B38" s="19">
@@ -8754,7 +8754,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="44"/>
+      <c r="A39" s="45"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -8793,7 +8793,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="44"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -8832,7 +8832,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="44"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -8871,7 +8871,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
+      <c r="A42" s="45"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -8910,7 +8910,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="45" t="s">
         <v>86</v>
       </c>
       <c r="B43" s="23">
@@ -8954,7 +8954,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="44"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -8996,7 +8996,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="44"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -9038,7 +9038,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="44"/>
+      <c r="A46" s="45"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -9080,7 +9080,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="44"/>
+      <c r="A47" s="45"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -9122,7 +9122,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="44"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -9200,7 +9200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB93F79-F640-47DC-B202-CD46132620C4}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
@@ -9684,15 +9684,15 @@
       <c r="G23" s="39">
         <v>273.919915629147</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="40">
@@ -11380,22 +11380,22 @@
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B103" s="51">
+      <c r="B103" s="44">
         <v>4.5390360000000003</v>
       </c>
-      <c r="C103" s="51">
+      <c r="C103" s="44">
         <v>12.703390000000001</v>
       </c>
-      <c r="D103" s="51">
+      <c r="D103" s="44">
         <v>13.09676</v>
       </c>
-      <c r="E103" s="51">
+      <c r="E103" s="44">
         <v>34.68338</v>
       </c>
-      <c r="F103" s="51">
+      <c r="F103" s="44">
         <v>123.28440000000001</v>
       </c>
-      <c r="G103" s="51">
+      <c r="G103" s="44">
         <v>190.18340000000001</v>
       </c>
     </row>
@@ -11481,6 +11481,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="O30:P30"/>
@@ -11490,19 +11503,6 @@
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="O29:P29"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -35211,19 +35211,19 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="50"/>
+      <c r="A108" s="51"/>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="50"/>
+      <c r="A109" s="51"/>
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="50"/>
+      <c r="A110" s="51"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="50"/>
+      <c r="A111" s="51"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="50"/>
+      <c r="A112" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -35237,8 +35237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5424DAFC-E75A-4FCC-BF86-3B2985A5EFC4}">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35277,7 +35277,9 @@
       <c r="B2" s="27">
         <v>86.215717286957002</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="27">
+        <v>0.61000000000200005</v>
+      </c>
       <c r="D2" s="27">
         <v>0.61000000000200005</v>
       </c>
@@ -35292,7 +35294,9 @@
       <c r="B3" s="27">
         <v>255.46977926144399</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="27">
+        <v>11.593756709989</v>
+      </c>
       <c r="D3" s="27">
         <v>300.39246636701301</v>
       </c>
@@ -35307,7 +35311,9 @@
       <c r="B4" s="27">
         <v>322.825426505537</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="27">
+        <v>0.86649636027200005</v>
+      </c>
       <c r="D4" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -35322,7 +35328,9 @@
       <c r="B5" s="27">
         <v>69.234275614509002</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="27">
+        <v>75.863795972847996</v>
+      </c>
       <c r="D5" s="27">
         <v>21.028171343808001</v>
       </c>
@@ -35337,7 +35345,9 @@
       <c r="B6" s="27">
         <v>0.71166666666900003</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="27">
+        <v>19.352795448138</v>
+      </c>
       <c r="D6" s="27">
         <v>255.02887362716399</v>
       </c>
@@ -35352,7 +35362,9 @@
       <c r="B7" s="27">
         <v>199.385199116786</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="27">
+        <v>88.921595770413006</v>
+      </c>
       <c r="D7" s="27">
         <v>194.52990985327301</v>
       </c>
@@ -35367,7 +35379,9 @@
       <c r="B8" s="27">
         <v>37.819968938732998</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="27">
+        <v>36.779670297091997</v>
+      </c>
       <c r="D8" s="27">
         <v>309.078285744276</v>
       </c>
@@ -35382,7 +35396,9 @@
       <c r="B9" s="27">
         <v>129.685999837</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="27">
+        <v>112.89930831452401</v>
+      </c>
       <c r="D9" s="27">
         <v>99.328049055614002</v>
       </c>
@@ -35397,7 +35413,9 @@
       <c r="B10" s="27">
         <v>209.44949922557001</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="27">
+        <v>6.3122088544189996</v>
+      </c>
       <c r="D10" s="27">
         <v>147.45127369990101</v>
       </c>
@@ -35412,7 +35430,9 @@
       <c r="B11" s="27">
         <v>23.764182685529001</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="27">
+        <v>66.519587813550999</v>
+      </c>
       <c r="D11" s="27">
         <v>315.41864572255002</v>
       </c>
@@ -35427,7 +35447,9 @@
       <c r="B12" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="27">
+        <v>54.684308815525</v>
+      </c>
       <c r="D12" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -35442,7 +35464,9 @@
       <c r="B13" s="27">
         <v>81.648809430669004</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="27">
+        <v>13.987861085325999</v>
+      </c>
       <c r="D13" s="27">
         <v>0.50833333333499997</v>
       </c>
@@ -35457,7 +35481,9 @@
       <c r="B14" s="27">
         <v>115.992972571278</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="27">
+        <v>48.075955851521996</v>
+      </c>
       <c r="D14" s="27">
         <v>281.69683473526197</v>
       </c>
@@ -35472,7 +35498,9 @@
       <c r="B15" s="27">
         <v>0.71166666666900003</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="27">
+        <v>51.075726164271998</v>
+      </c>
       <c r="D15" s="27">
         <v>231.001774693523</v>
       </c>
@@ -35487,7 +35515,9 @@
       <c r="B16" s="27">
         <v>307.13115937735</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="27">
+        <v>29.405147852654</v>
+      </c>
       <c r="D16" s="27">
         <v>307.46930563203301</v>
       </c>
@@ -35502,7 +35532,9 @@
       <c r="B17" s="27">
         <v>86.298118854934998</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="27">
+        <v>77.396274284151005</v>
+      </c>
       <c r="D17" s="27">
         <v>259.70001892298001</v>
       </c>
@@ -35517,7 +35549,9 @@
       <c r="B18" s="27">
         <v>120.214659101637</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="27">
+        <v>81.528373187594994</v>
+      </c>
       <c r="D18" s="27">
         <v>228.65130824048501</v>
       </c>
@@ -35532,7 +35566,9 @@
       <c r="B19" s="27">
         <v>300.25839351607999</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="27">
+        <v>12.910569999722</v>
+      </c>
       <c r="D19" s="27">
         <v>200.80574640533899</v>
       </c>
@@ -35547,7 +35583,9 @@
       <c r="B20" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="27">
+        <v>41.065432958880002</v>
+      </c>
       <c r="D20" s="27">
         <v>39.624787672372001</v>
       </c>
@@ -35562,7 +35600,9 @@
       <c r="B21" s="27">
         <v>44.142613464</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="27">
+        <v>10.523896334756</v>
+      </c>
       <c r="D21" s="27">
         <v>448.63439339754302</v>
       </c>
@@ -35577,7 +35617,9 @@
       <c r="B22" s="27">
         <v>161.25911196069501</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="27">
+        <v>46.094404766670998</v>
+      </c>
       <c r="D22" s="27">
         <v>71.876092155739002</v>
       </c>
@@ -35592,7 +35634,9 @@
       <c r="B23" s="27">
         <v>111.94315110734399</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="27">
+        <v>23.747226358528</v>
+      </c>
       <c r="D23" s="27">
         <v>133.53160691106001</v>
       </c>
@@ -35607,7 +35651,9 @@
       <c r="B24" s="27">
         <v>0.71166666666900003</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="C24" s="27">
+        <v>66.416724657215994</v>
+      </c>
       <c r="D24" s="27">
         <v>374.56493702683201</v>
       </c>
@@ -35622,7 +35668,9 @@
       <c r="B25" s="27">
         <v>126.86806141703001</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="27">
+        <v>67.245366141459002</v>
+      </c>
       <c r="D25" s="27">
         <v>362.682062005445</v>
       </c>
@@ -35637,7 +35685,9 @@
       <c r="B26" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C26" s="27"/>
+      <c r="C26" s="27">
+        <v>42.717558737764001</v>
+      </c>
       <c r="D26" s="27">
         <v>115.432041621915</v>
       </c>
@@ -35652,7 +35702,9 @@
       <c r="B27" s="27">
         <v>78.774905857158004</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="27">
+        <v>8.4901085824900004</v>
+      </c>
       <c r="D27" s="27">
         <v>353.26345850330398</v>
       </c>
@@ -35667,7 +35719,9 @@
       <c r="B28" s="27">
         <v>108.13198920841199</v>
       </c>
-      <c r="C28" s="27"/>
+      <c r="C28" s="27">
+        <v>10.490394260793</v>
+      </c>
       <c r="D28" s="27">
         <v>634.14088039084004</v>
       </c>
@@ -35682,7 +35736,9 @@
       <c r="B29" s="27">
         <v>56.027205100482</v>
       </c>
-      <c r="C29" s="27"/>
+      <c r="C29" s="27">
+        <v>33.546325682366003</v>
+      </c>
       <c r="D29" s="27">
         <v>149.815072372754</v>
       </c>
@@ -35697,7 +35753,9 @@
       <c r="B30" s="27">
         <v>194.187444201452</v>
       </c>
-      <c r="C30" s="27"/>
+      <c r="C30" s="27">
+        <v>6.0177619760420002</v>
+      </c>
       <c r="D30" s="27">
         <v>92.022306482888993</v>
       </c>
@@ -35712,7 +35770,9 @@
       <c r="B31" s="27">
         <v>7.7827416201619997</v>
       </c>
-      <c r="C31" s="27"/>
+      <c r="C31" s="27">
+        <v>11.956429364206</v>
+      </c>
       <c r="D31" s="27">
         <v>893.77595961272402</v>
       </c>
@@ -35727,7 +35787,9 @@
       <c r="B32" s="27">
         <v>313.69824254259498</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>14.228133743226</v>
+      </c>
       <c r="D32" s="27">
         <v>197.282867034688</v>
       </c>
@@ -35742,7 +35804,9 @@
       <c r="B33" s="27">
         <v>146.06299727923201</v>
       </c>
-      <c r="C33" s="27"/>
+      <c r="C33" s="27">
+        <v>2.0423967040390001</v>
+      </c>
       <c r="D33" s="27">
         <v>51.993088404289999</v>
       </c>
@@ -35757,7 +35821,9 @@
       <c r="B34" s="27">
         <v>170.62334172113401</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="27">
+        <v>0.813333333336</v>
+      </c>
       <c r="D34" s="27">
         <v>83.666561216391003</v>
       </c>
@@ -35772,7 +35838,9 @@
       <c r="B35" s="27">
         <v>77.852640581653006</v>
       </c>
-      <c r="C35" s="27"/>
+      <c r="C35" s="27">
+        <v>70.774229407248001</v>
+      </c>
       <c r="D35" s="27">
         <v>0.61000000000200005</v>
       </c>
@@ -35787,7 +35855,9 @@
       <c r="B36" s="27">
         <v>180.721535415555</v>
       </c>
-      <c r="C36" s="27"/>
+      <c r="C36" s="27">
+        <v>28.201257043696</v>
+      </c>
       <c r="D36" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -35802,7 +35872,9 @@
       <c r="B37" s="27">
         <v>12.432291170022999</v>
       </c>
-      <c r="C37" s="27"/>
+      <c r="C37" s="27">
+        <v>48.999238651291002</v>
+      </c>
       <c r="D37" s="27">
         <v>113.03551863726901</v>
       </c>
@@ -35817,7 +35889,9 @@
       <c r="B38" s="27">
         <v>29.683793238671999</v>
       </c>
-      <c r="C38" s="27"/>
+      <c r="C38" s="27">
+        <v>46.223911001437997</v>
+      </c>
       <c r="D38" s="27">
         <v>114.54803046152701</v>
       </c>
@@ -35832,7 +35906,9 @@
       <c r="B39" s="27">
         <v>173.70522988131199</v>
       </c>
-      <c r="C39" s="27"/>
+      <c r="C39" s="27">
+        <v>46.255574055821</v>
+      </c>
       <c r="D39" s="27">
         <v>178.278454527875</v>
       </c>
@@ -35847,7 +35923,9 @@
       <c r="B40" s="27">
         <v>116.02174339932</v>
       </c>
-      <c r="C40" s="27"/>
+      <c r="C40" s="27">
+        <v>45.625446842565999</v>
+      </c>
       <c r="D40" s="27">
         <v>212.48645845994801</v>
       </c>
@@ -35862,7 +35940,9 @@
       <c r="B41" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C41" s="27"/>
+      <c r="C41" s="27">
+        <v>35.115699312495998</v>
+      </c>
       <c r="D41" s="27">
         <v>7.3428763474260004</v>
       </c>
@@ -35877,7 +35957,9 @@
       <c r="B42" s="27">
         <v>30.251465077155</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="27">
+        <v>45.984775340544999</v>
+      </c>
       <c r="D42" s="27">
         <v>209.683036945449</v>
       </c>
@@ -35892,7 +35974,9 @@
       <c r="B43" s="27">
         <v>77.138866736262997</v>
       </c>
-      <c r="C43" s="27"/>
+      <c r="C43" s="27">
+        <v>39.861097918115</v>
+      </c>
       <c r="D43" s="27">
         <v>221.64830439998701</v>
       </c>
@@ -35907,7 +35991,9 @@
       <c r="B44" s="27">
         <v>61.332128247425999</v>
       </c>
-      <c r="C44" s="27"/>
+      <c r="C44" s="27">
+        <v>46.499010403370001</v>
+      </c>
       <c r="D44" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -35922,7 +36008,9 @@
       <c r="B45" s="27">
         <v>19.106546880142002</v>
       </c>
-      <c r="C45" s="27"/>
+      <c r="C45" s="27">
+        <v>39.140731299273</v>
+      </c>
       <c r="D45" s="27">
         <v>241.545721069725</v>
       </c>
@@ -35937,7 +36025,9 @@
       <c r="B46" s="27">
         <v>0.406666666668</v>
       </c>
-      <c r="C46" s="27"/>
+      <c r="C46" s="27">
+        <v>28.963919475586</v>
+      </c>
       <c r="D46" s="27">
         <v>138.82913162444001</v>
       </c>
@@ -35952,7 +36042,9 @@
       <c r="B47" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C47" s="27"/>
+      <c r="C47" s="27">
+        <v>28.476086812011001</v>
+      </c>
       <c r="D47" s="27">
         <v>305.84402966943799</v>
       </c>
@@ -35967,7 +36059,9 @@
       <c r="B48" s="27">
         <v>52.969990464481</v>
       </c>
-      <c r="C48" s="27"/>
+      <c r="C48" s="27">
+        <v>96.249764419086006</v>
+      </c>
       <c r="D48" s="27">
         <v>105.82907320763201</v>
       </c>
@@ -35982,7 +36076,9 @@
       <c r="B49" s="27">
         <v>3.4685687493009998</v>
       </c>
-      <c r="C49" s="27"/>
+      <c r="C49" s="27">
+        <v>20.259153224647001</v>
+      </c>
       <c r="D49" s="27">
         <v>82.074562108552001</v>
       </c>
@@ -35997,7 +36093,9 @@
       <c r="B50" s="27">
         <v>145.765407901153</v>
       </c>
-      <c r="C50" s="27"/>
+      <c r="C50" s="27">
+        <v>27.603310016859002</v>
+      </c>
       <c r="D50" s="27">
         <v>234.57061278329601</v>
       </c>
@@ -36012,7 +36110,9 @@
       <c r="B51" s="27">
         <v>129.538620617486</v>
       </c>
-      <c r="C51" s="27"/>
+      <c r="C51" s="27">
+        <v>87.827832195363001</v>
+      </c>
       <c r="D51" s="27">
         <v>167.30992538279099</v>
       </c>
@@ -36027,7 +36127,9 @@
       <c r="B52" s="27">
         <v>171.690615719466</v>
       </c>
-      <c r="C52" s="27"/>
+      <c r="C52" s="27">
+        <v>32.480374303742998</v>
+      </c>
       <c r="D52" s="27">
         <v>177.41963794589299</v>
       </c>
@@ -36042,7 +36144,9 @@
       <c r="B53" s="27">
         <v>152.34079044330201</v>
       </c>
-      <c r="C53" s="27"/>
+      <c r="C53" s="27">
+        <v>90.851330165868006</v>
+      </c>
       <c r="D53" s="27">
         <v>501.79753336436698</v>
       </c>
@@ -36057,7 +36161,9 @@
       <c r="B54" s="27">
         <v>207.19953969573999</v>
       </c>
-      <c r="C54" s="27"/>
+      <c r="C54" s="27">
+        <v>56.041463061601</v>
+      </c>
       <c r="D54" s="27">
         <v>615.51698065588403</v>
       </c>
@@ -36072,7 +36178,9 @@
       <c r="B55" s="27">
         <v>18.120606428485999</v>
       </c>
-      <c r="C55" s="27"/>
+      <c r="C55" s="27">
+        <v>11.583028498795001</v>
+      </c>
       <c r="D55" s="27">
         <v>480.25559654358</v>
       </c>
@@ -36087,7 +36195,9 @@
       <c r="B56" s="27">
         <v>0.50833333333499997</v>
       </c>
-      <c r="C56" s="27"/>
+      <c r="C56" s="27">
+        <v>52.273470529359003</v>
+      </c>
       <c r="D56" s="27">
         <v>0.61000000000200005</v>
       </c>
@@ -36102,7 +36212,9 @@
       <c r="B57" s="27">
         <v>75.880794247291007</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="27">
+        <v>85.552043020409002</v>
+      </c>
       <c r="D57" s="27">
         <v>175.032595356874</v>
       </c>
@@ -36117,7 +36229,9 @@
       <c r="B58" s="27">
         <v>71.575781775479996</v>
       </c>
-      <c r="C58" s="27"/>
+      <c r="C58" s="27">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="D58" s="27">
         <v>80.666183831604997</v>
       </c>
@@ -36132,7 +36246,9 @@
       <c r="B59" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C59" s="27"/>
+      <c r="C59" s="27">
+        <v>10.939050040665</v>
+      </c>
       <c r="D59" s="27">
         <v>285.28929946200901</v>
       </c>
@@ -36147,7 +36263,9 @@
       <c r="B60" s="27">
         <v>26.100401725615999</v>
       </c>
-      <c r="C60" s="27"/>
+      <c r="C60" s="27">
+        <v>2.8854085839739998</v>
+      </c>
       <c r="D60" s="27">
         <v>136.43117826592601</v>
       </c>
@@ -36162,7 +36280,9 @@
       <c r="B61" s="27">
         <v>39.854453799505997</v>
       </c>
-      <c r="C61" s="27"/>
+      <c r="C61" s="27">
+        <v>135.01677903229299</v>
+      </c>
       <c r="D61" s="27">
         <v>342.16820468256901</v>
       </c>
@@ -36177,7 +36297,9 @@
       <c r="B62" s="27">
         <v>228.07340261079199</v>
       </c>
-      <c r="C62" s="27"/>
+      <c r="C62" s="27">
+        <v>78.214714470008005</v>
+      </c>
       <c r="D62" s="27">
         <v>49.197089089160997</v>
       </c>
@@ -36192,7 +36314,9 @@
       <c r="B63" s="27">
         <v>153.31536741932899</v>
       </c>
-      <c r="C63" s="27"/>
+      <c r="C63" s="27">
+        <v>83.014953693495997</v>
+      </c>
       <c r="D63" s="27">
         <v>26.454536634943</v>
       </c>
@@ -36207,7 +36331,9 @@
       <c r="B64" s="27">
         <v>81.461409288278006</v>
       </c>
-      <c r="C64" s="27"/>
+      <c r="C64" s="27">
+        <v>28.123571075417999</v>
+      </c>
       <c r="D64" s="27">
         <v>351.077979251697</v>
       </c>
@@ -36222,7 +36348,9 @@
       <c r="B65" s="27">
         <v>99.573041634812995</v>
       </c>
-      <c r="C65" s="27"/>
+      <c r="C65" s="27">
+        <v>26.342666351719</v>
+      </c>
       <c r="D65" s="27">
         <v>536.27508083275302</v>
       </c>
@@ -36237,7 +36365,9 @@
       <c r="B66" s="27">
         <v>175.53225995288901</v>
       </c>
-      <c r="C66" s="27"/>
+      <c r="C66" s="27">
+        <v>42.094544693830997</v>
+      </c>
       <c r="D66" s="27">
         <v>528.116396105842</v>
       </c>
@@ -36252,7 +36382,9 @@
       <c r="B67" s="27">
         <v>106.605827394811</v>
       </c>
-      <c r="C67" s="27"/>
+      <c r="C67" s="27">
+        <v>98.629688767662998</v>
+      </c>
       <c r="D67" s="27">
         <v>264.89144272808898</v>
       </c>
@@ -36267,7 +36399,9 @@
       <c r="B68" s="27">
         <v>82.269516669469994</v>
       </c>
-      <c r="C68" s="27"/>
+      <c r="C68" s="27">
+        <v>4.808706338176</v>
+      </c>
       <c r="D68" s="27">
         <v>74.341679629449999</v>
       </c>
@@ -36282,7 +36416,9 @@
       <c r="B69" s="27">
         <v>48.206584728757001</v>
       </c>
-      <c r="C69" s="27"/>
+      <c r="C69" s="27">
+        <v>3.2793289687330001</v>
+      </c>
       <c r="D69" s="27">
         <v>57.864758695454</v>
       </c>
@@ -36297,7 +36433,9 @@
       <c r="B70" s="27">
         <v>229.87883781267601</v>
       </c>
-      <c r="C70" s="27"/>
+      <c r="C70" s="27">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="D70" s="27">
         <v>71.702678275701999</v>
       </c>
@@ -36312,7 +36450,9 @@
       <c r="B71" s="27">
         <v>93.983183833268995</v>
       </c>
-      <c r="C71" s="27"/>
+      <c r="C71" s="27">
+        <v>89.965426356399007</v>
+      </c>
       <c r="D71" s="27">
         <v>49.602413367581001</v>
       </c>
@@ -36327,7 +36467,9 @@
       <c r="B72" s="27">
         <v>27.457045426202999</v>
       </c>
-      <c r="C72" s="27"/>
+      <c r="C72" s="27">
+        <v>35.486521995746998</v>
+      </c>
       <c r="D72" s="27">
         <v>4.2062114438889999</v>
       </c>
@@ -36342,7 +36484,9 @@
       <c r="B73" s="27">
         <v>42.649244335311998</v>
       </c>
-      <c r="C73" s="27"/>
+      <c r="C73" s="27">
+        <v>50.842261506900002</v>
+      </c>
       <c r="D73" s="27">
         <v>219.95960791207801</v>
       </c>
@@ -36357,7 +36501,9 @@
       <c r="B74" s="27">
         <v>191.79417212995</v>
       </c>
-      <c r="C74" s="27"/>
+      <c r="C74" s="27">
+        <v>26.757684977823001</v>
+      </c>
       <c r="D74" s="27">
         <v>22.785214715717</v>
       </c>
@@ -36372,7 +36518,9 @@
       <c r="B75" s="27">
         <v>50.331375417376996</v>
       </c>
-      <c r="C75" s="27"/>
+      <c r="C75" s="27">
+        <v>90.266999378540007</v>
+      </c>
       <c r="D75" s="27">
         <v>327.74208368573801</v>
       </c>
@@ -36387,7 +36535,9 @@
       <c r="B76" s="27">
         <v>12.687165395728</v>
       </c>
-      <c r="C76" s="27"/>
+      <c r="C76" s="27">
+        <v>64.224069604609994</v>
+      </c>
       <c r="D76" s="27">
         <v>0.50833333333499997</v>
       </c>
@@ -36402,7 +36552,9 @@
       <c r="B77" s="27">
         <v>23.663825388486</v>
       </c>
-      <c r="C77" s="27"/>
+      <c r="C77" s="27">
+        <v>9.2909756240450001</v>
+      </c>
       <c r="D77" s="27">
         <v>54.285426229805999</v>
       </c>
@@ -36417,7 +36569,9 @@
       <c r="B78" s="27">
         <v>247.959445503403</v>
       </c>
-      <c r="C78" s="27"/>
+      <c r="C78" s="27">
+        <v>25.933032698866</v>
+      </c>
       <c r="D78" s="27">
         <v>445.14250390198401</v>
       </c>
@@ -36432,7 +36586,9 @@
       <c r="B79" s="27">
         <v>90.097345550173003</v>
       </c>
-      <c r="C79" s="27"/>
+      <c r="C79" s="27">
+        <v>105.276026116683</v>
+      </c>
       <c r="D79" s="27">
         <v>284.23930936026397</v>
       </c>
@@ -36447,7 +36603,9 @@
       <c r="B80" s="27">
         <v>252.726050883483</v>
       </c>
-      <c r="C80" s="27"/>
+      <c r="C80" s="27">
+        <v>62.004319454410002</v>
+      </c>
       <c r="D80" s="27">
         <v>124.245578489482</v>
       </c>
@@ -36462,7 +36620,9 @@
       <c r="B81" s="27">
         <v>211.99082290560901</v>
       </c>
-      <c r="C81" s="27"/>
+      <c r="C81" s="27">
+        <v>63.029265233548003</v>
+      </c>
       <c r="D81" s="27">
         <v>95.607599907804996</v>
       </c>
@@ -36477,7 +36637,9 @@
       <c r="B82" s="27">
         <v>144.19439684610501</v>
       </c>
-      <c r="C82" s="27"/>
+      <c r="C82" s="27">
+        <v>56.140909154306001</v>
+      </c>
       <c r="D82" s="27">
         <v>133.804334560527</v>
       </c>
@@ -36492,7 +36654,9 @@
       <c r="B83" s="27">
         <v>200.09620921494101</v>
       </c>
-      <c r="C83" s="27"/>
+      <c r="C83" s="27">
+        <v>92.415386798141</v>
+      </c>
       <c r="D83" s="27">
         <v>177.38363761322901</v>
       </c>
@@ -36507,7 +36671,9 @@
       <c r="B84" s="27">
         <v>129.15303936333899</v>
       </c>
-      <c r="C84" s="27"/>
+      <c r="C84" s="27">
+        <v>0.406666666668</v>
+      </c>
       <c r="D84" s="27">
         <v>444.43231517404899</v>
       </c>
@@ -36522,7 +36688,9 @@
       <c r="B85" s="27">
         <v>99.861862251408994</v>
       </c>
-      <c r="C85" s="27"/>
+      <c r="C85" s="27">
+        <v>3.2418018693940001</v>
+      </c>
       <c r="D85" s="27">
         <v>341.24698278209399</v>
       </c>
@@ -36537,7 +36705,9 @@
       <c r="B86" s="27">
         <v>8.4567001590869992</v>
       </c>
-      <c r="C86" s="27"/>
+      <c r="C86" s="27">
+        <v>87.059661917441005</v>
+      </c>
       <c r="D86" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -36552,7 +36722,9 @@
       <c r="B87" s="27">
         <v>267.72584732016003</v>
       </c>
-      <c r="C87" s="27"/>
+      <c r="C87" s="27">
+        <v>22.585100746925001</v>
+      </c>
       <c r="D87" s="27">
         <v>88.132088082832993</v>
       </c>
@@ -36567,7 +36739,9 @@
       <c r="B88" s="27">
         <v>68.597646721645006</v>
       </c>
-      <c r="C88" s="27"/>
+      <c r="C88" s="27">
+        <v>53.736180347553997</v>
+      </c>
       <c r="D88" s="27">
         <v>241.019350453779</v>
       </c>
@@ -36582,7 +36756,9 @@
       <c r="B89" s="27">
         <v>3.147917961463</v>
       </c>
-      <c r="C89" s="27"/>
+      <c r="C89" s="27">
+        <v>11.512294073834999</v>
+      </c>
       <c r="D89" s="27">
         <v>0.61000000000200005</v>
       </c>
@@ -36597,7 +36773,9 @@
       <c r="B90" s="27">
         <v>68.116402788974</v>
       </c>
-      <c r="C90" s="27"/>
+      <c r="C90" s="27">
+        <v>67.966023823265999</v>
+      </c>
       <c r="D90" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -36612,7 +36790,9 @@
       <c r="B91" s="27">
         <v>1.3583558640719999</v>
       </c>
-      <c r="C91" s="27"/>
+      <c r="C91" s="27">
+        <v>36.370448547228001</v>
+      </c>
       <c r="D91" s="27">
         <v>100.246251731475</v>
       </c>
@@ -36627,7 +36807,9 @@
       <c r="B92" s="27">
         <v>44.743075345645998</v>
       </c>
-      <c r="C92" s="27"/>
+      <c r="C92" s="27">
+        <v>58.145127427189003</v>
+      </c>
       <c r="D92" s="27">
         <v>150.50886036926499</v>
       </c>
@@ -36642,7 +36824,9 @@
       <c r="B93" s="27">
         <v>128.18918365888101</v>
       </c>
-      <c r="C93" s="27"/>
+      <c r="C93" s="27">
+        <v>0.61000000000200005</v>
+      </c>
       <c r="D93" s="27">
         <v>212.03886796944801</v>
       </c>
@@ -36657,7 +36841,9 @@
       <c r="B94" s="27">
         <v>45.218614879425999</v>
       </c>
-      <c r="C94" s="27"/>
+      <c r="C94" s="27">
+        <v>2.762635045588</v>
+      </c>
       <c r="D94" s="27">
         <v>45.374419549952997</v>
       </c>
@@ -36672,7 +36858,9 @@
       <c r="B95" s="27">
         <v>73.425982738692994</v>
       </c>
-      <c r="C95" s="27"/>
+      <c r="C95" s="27">
+        <v>44.579799203038</v>
+      </c>
       <c r="D95" s="27">
         <v>139.45984377282599</v>
       </c>
@@ -36687,7 +36875,9 @@
       <c r="B96" s="27">
         <v>0.813333333336</v>
       </c>
-      <c r="C96" s="27"/>
+      <c r="C96" s="27">
+        <v>8.8422179309400004</v>
+      </c>
       <c r="D96" s="27">
         <v>505.21337718676199</v>
       </c>
@@ -36702,7 +36892,9 @@
       <c r="B97" s="27">
         <v>92.161697096734997</v>
       </c>
-      <c r="C97" s="27"/>
+      <c r="C97" s="27">
+        <v>57.523571559181001</v>
+      </c>
       <c r="D97" s="27">
         <v>632.37611586544904</v>
       </c>
@@ -36717,7 +36909,9 @@
       <c r="B98" s="27">
         <v>103.398465921011</v>
       </c>
-      <c r="C98" s="27"/>
+      <c r="C98" s="27">
+        <v>34.030091277182002</v>
+      </c>
       <c r="D98" s="27">
         <v>0.71166666666900003</v>
       </c>
@@ -36732,7 +36926,9 @@
       <c r="B99" s="27">
         <v>124.41775923873099</v>
       </c>
-      <c r="C99" s="27"/>
+      <c r="C99" s="27">
+        <v>0.71166666666900003</v>
+      </c>
       <c r="D99" s="27">
         <v>95.455855567854996</v>
       </c>
@@ -36747,7 +36943,9 @@
       <c r="B100" s="27">
         <v>0.61000000000200005</v>
       </c>
-      <c r="C100" s="27"/>
+      <c r="C100" s="27">
+        <v>91.337532504498</v>
+      </c>
       <c r="D100" s="27">
         <v>225.99732233329601</v>
       </c>
@@ -36762,7 +36960,9 @@
       <c r="B101" s="27">
         <v>279.36092210862301</v>
       </c>
-      <c r="C101" s="27"/>
+      <c r="C101" s="27">
+        <v>26.114033397278</v>
+      </c>
       <c r="D101" s="27">
         <v>317.31336652359801</v>
       </c>
@@ -36784,7 +36984,9 @@
       <c r="B103" s="27">
         <v>100.7766</v>
       </c>
-      <c r="C103" s="27"/>
+      <c r="C103" s="27">
+        <v>41.789619999999999</v>
+      </c>
       <c r="D103" s="27">
         <v>197.27670000000001</v>
       </c>
@@ -36799,7 +37001,9 @@
       <c r="B104" s="27">
         <v>86.271680000000003</v>
       </c>
-      <c r="C104" s="27"/>
+      <c r="C104" s="27">
+        <v>31.640889999999999</v>
+      </c>
       <c r="D104" s="27">
         <v>175.05529999999999</v>
       </c>
@@ -36814,7 +37018,9 @@
       <c r="B105" s="27">
         <v>16.908940000000001</v>
       </c>
-      <c r="C105" s="27"/>
+      <c r="C105" s="27">
+        <v>6.2015010000000004</v>
+      </c>
       <c r="D105" s="27">
         <v>34.310200000000002</v>
       </c>
@@ -36829,7 +37035,9 @@
       <c r="B106" s="27">
         <v>4</v>
       </c>
-      <c r="C106" s="27"/>
+      <c r="C106" s="27">
+        <v>0</v>
+      </c>
       <c r="D106" s="27">
         <v>4</v>
       </c>
@@ -36844,7 +37052,9 @@
       <c r="B107" s="27">
         <v>96</v>
       </c>
-      <c r="C107" s="27"/>
+      <c r="C107" s="27">
+        <v>100</v>
+      </c>
       <c r="D107" s="27">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
added simulation results for networks of 5k nodes
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 0.xlsx
+++ b/Data Collections/Data Collection Sim 0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\Data Collections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0845A7F5-DB18-4663-B97A-43B5FA032FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895527FE-DF80-42CB-B17A-D5A318570F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4656" yWindow="1776" windowWidth="17280" windowHeight="9024" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -591,7 +591,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,6 +664,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -676,10 +680,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -7053,11 +7057,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B34" sqref="A34:XFD34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7132,7 +7136,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="4">
@@ -7176,7 +7180,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -7188,7 +7192,7 @@
         <v>0.13695052585936646</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E41" si="0">LN(C3)/(C3)</f>
+        <f t="shared" ref="E3:E42" si="0">LN(C3)/(C3)</f>
         <v>0.14978661367769955</v>
       </c>
       <c r="F3" s="1">
@@ -7218,7 +7222,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -7226,7 +7230,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D37" si="1">2*LOG(C4)/(C4-1)</f>
+        <f t="shared" ref="D4:D38" si="1">2*LOG(C4)/(C4-1)</f>
         <v>6.9345714462694649E-2</v>
       </c>
       <c r="E4" s="1">
@@ -7262,7 +7266,7 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -7305,7 +7309,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -7349,7 +7353,7 @@
       <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -7392,71 +7396,46 @@
       </c>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
+    <row r="8" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="47"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="45">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="T8" s="45"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>10000</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>8.0008000800080011E-4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>9.210340371976184E-4</v>
       </c>
-      <c r="F8" s="26">
-        <f>E8</f>
+      <c r="F9" s="26">
+        <f>E9</f>
         <v>9.210340371976184E-4</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>100</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="26">
-        <v>100</v>
-      </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>500</v>
-      </c>
-      <c r="D9" s="1">
-        <f>2*LOG(C9)/(C9-1)</f>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E9" s="1">
-        <f>LN(C9)/(C9)</f>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F9" s="28">
-        <f>E9</f>
-        <v>1.2429216196844383E-2</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="1">
@@ -7483,11 +7462,13 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
+      <c r="A10" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="26">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>500</v>
       </c>
       <c r="D10" s="1">
@@ -7499,7 +7480,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F10" s="28">
-        <f t="shared" ref="F10:F37" si="3">E10</f>
+        <f>E10</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G10" s="18"/>
@@ -7510,7 +7491,7 @@
         <v>100</v>
       </c>
       <c r="J10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>8</v>
@@ -7526,24 +7507,24 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
       <c r="B11" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="26">
         <v>500</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f>2*LOG(C11)/(C11-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f>LN(C11)/(C11)</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F11" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F11:F38" si="3">E11</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G11" s="18"/>
@@ -7554,7 +7535,7 @@
         <v>100</v>
       </c>
       <c r="J11" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>8</v>
@@ -7571,18 +7552,18 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="26">
         <v>500</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
@@ -7590,45 +7571,43 @@
         <f t="shared" si="3"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="28">
+      <c r="G12" s="18"/>
+      <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="1">
         <v>100</v>
       </c>
-      <c r="J12" s="22">
-        <v>20</v>
-      </c>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="1">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="N12" s="26">
         <v>100</v>
       </c>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="28">
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="26">
         <v>500</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="22">
         <f t="shared" si="1"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="22">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
@@ -7636,33 +7615,36 @@
         <f t="shared" si="3"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="28">
         <v>1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="22">
         <v>100</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="22">
+        <v>20</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="26">
+        <v>100</v>
+      </c>
+      <c r="T13" s="22"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6">
         <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="6">
-        <v>2</v>
       </c>
       <c r="C14" s="28">
         <v>500</v>
@@ -7693,7 +7675,7 @@
         <v>8</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>10</v>
@@ -7703,9 +7685,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="28">
         <v>500</v>
@@ -7736,7 +7718,7 @@
         <v>8</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>10</v>
@@ -7746,9 +7728,9 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="28">
         <v>500</v>
@@ -7779,7 +7761,7 @@
         <v>8</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>10</v>
@@ -7789,9 +7771,9 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="28">
         <v>500</v>
@@ -7822,7 +7804,7 @@
         <v>8</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>10</v>
@@ -7832,9 +7814,9 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="28">
         <v>500</v>
@@ -7865,7 +7847,7 @@
         <v>8</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>10</v>
@@ -7874,12 +7856,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="6">
+        <v>6</v>
       </c>
       <c r="C19" s="28">
         <v>500</v>
@@ -7910,30 +7890,30 @@
         <v>8</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="28">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="29">
+    <row r="20" spans="1:16" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8">
         <v>1</v>
       </c>
       <c r="C20" s="28">
         <v>500</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="1">
         <f t="shared" si="1"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
@@ -7941,37 +7921,35 @@
         <f t="shared" si="3"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="28">
         <v>1</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="1">
         <v>100</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="1">
         <v>1</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="L20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="29">
         <v>1</v>
-      </c>
-      <c r="O20" s="31"/>
-      <c r="P20" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="29">
-        <v>2</v>
       </c>
       <c r="C21" s="28">
         <v>500</v>
@@ -8012,24 +7990,22 @@
       </c>
       <c r="O21" s="31"/>
       <c r="P21" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="10">
-        <v>1</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50"/>
+      <c r="B22" s="29">
+        <v>2</v>
       </c>
       <c r="C22" s="28">
         <v>500</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="30">
         <f t="shared" si="1"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="30">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
@@ -8037,33 +8013,39 @@
         <f t="shared" si="3"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G22" s="18"/>
+      <c r="G22" s="30"/>
       <c r="H22" s="28">
         <v>1</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="30">
         <v>100</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="30">
         <v>1</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="M22" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N22" s="1">
-        <v>100</v>
+      <c r="N22" s="30">
+        <v>1</v>
+      </c>
+      <c r="O22" s="31"/>
+      <c r="P22" s="30" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
-      <c r="B23" s="11">
-        <v>2</v>
+      <c r="A23" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
       </c>
       <c r="C23" s="28">
         <v>500</v>
@@ -8091,7 +8073,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>7</v>
@@ -8104,9 +8086,9 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="45"/>
-      <c r="B24" s="10">
-        <v>3</v>
+      <c r="A24" s="47"/>
+      <c r="B24" s="11">
+        <v>2</v>
       </c>
       <c r="C24" s="28">
         <v>500</v>
@@ -8134,7 +8116,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>7</v>
@@ -8147,9 +8129,9 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="45"/>
-      <c r="B25" s="11">
-        <v>4</v>
+      <c r="A25" s="47"/>
+      <c r="B25" s="10">
+        <v>3</v>
       </c>
       <c r="C25" s="28">
         <v>500</v>
@@ -8177,7 +8159,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>7</v>
@@ -8190,9 +8172,9 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
-      <c r="B26" s="10">
-        <v>5</v>
+      <c r="A26" s="47"/>
+      <c r="B26" s="11">
+        <v>4</v>
       </c>
       <c r="C26" s="28">
         <v>500</v>
@@ -8220,7 +8202,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>7</v>
@@ -8233,17 +8215,15 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="12">
-        <v>1</v>
+      <c r="A27" s="47"/>
+      <c r="B27" s="10">
+        <v>5</v>
       </c>
       <c r="C27" s="28">
         <v>500</v>
       </c>
       <c r="D27" s="1">
-        <f>2*LOG(C27)/(C27-1)</f>
+        <f t="shared" si="1"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E27" s="1">
@@ -8255,7 +8235,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G27" s="18"/>
-      <c r="H27" s="1">
+      <c r="H27" s="28">
         <v>1</v>
       </c>
       <c r="I27" s="1">
@@ -8265,7 +8245,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>7</v>
@@ -8276,14 +8256,13 @@
       <c r="N27" s="1">
         <v>100</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="47" t="s">
+        <v>50</v>
+      </c>
       <c r="B28" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="28">
         <v>500</v>
@@ -8302,7 +8281,7 @@
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" s="1">
         <v>100</v>
@@ -8322,17 +8301,20 @@
       <c r="N28" s="1">
         <v>100</v>
       </c>
+      <c r="P28" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="45"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="28">
         <v>500</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
+        <f>2*LOG(C29)/(C29-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E29" s="1">
@@ -8345,7 +8327,7 @@
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1">
         <v>100</v>
@@ -8367,9 +8349,9 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="45"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="28">
         <v>500</v>
@@ -8388,7 +8370,7 @@
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1">
         <v>100</v>
@@ -8410,9 +8392,9 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="45"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="28">
         <v>500</v>
@@ -8431,7 +8413,7 @@
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I31" s="1">
         <v>100</v>
@@ -8453,9 +8435,9 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="28">
         <v>500</v>
@@ -8474,7 +8456,7 @@
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I32" s="1">
         <v>100</v>
@@ -8496,11 +8478,9 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="14">
-        <v>1</v>
+      <c r="A33" s="47"/>
+      <c r="B33" s="12">
+        <v>6</v>
       </c>
       <c r="C33" s="28">
         <v>500</v>
@@ -8519,7 +8499,7 @@
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="I33" s="1">
         <v>100</v>
@@ -8534,16 +8514,18 @@
         <v>7</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="N33" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="47" t="s">
+        <v>51</v>
+      </c>
       <c r="B34" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="28">
         <v>500</v>
@@ -8561,7 +8543,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G34" s="18"/>
-      <c r="H34" s="28">
+      <c r="H34" s="1">
         <v>1</v>
       </c>
       <c r="I34" s="1">
@@ -8577,16 +8559,16 @@
         <v>7</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N34" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="28">
         <v>500</v>
@@ -8620,16 +8602,16 @@
         <v>7</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N35" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="28">
         <v>500</v>
@@ -8663,16 +8645,16 @@
         <v>7</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N36" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="28">
         <v>500</v>
@@ -8706,59 +8688,63 @@
         <v>7</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N37" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="19">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="A38" s="47"/>
+      <c r="B38" s="14">
+        <v>5</v>
+      </c>
+      <c r="C38" s="28">
         <v>500</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="18">
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E38" s="1">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="18">
-        <v>1</v>
-      </c>
+      <c r="F38" s="28">
+        <f t="shared" si="3"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="G38" s="18"/>
       <c r="H38" s="28">
         <v>1</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="1">
         <v>100</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="1">
         <v>1</v>
       </c>
-      <c r="K38" s="18" t="s">
+      <c r="K38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="18" t="s">
+      <c r="L38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="24" t="s">
-        <v>10</v>
+      <c r="M38" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="N38" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="47" t="s">
+        <v>85</v>
+      </c>
       <c r="B39" s="19">
-        <v>2</v>
-      </c>
-      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
         <v>500</v>
       </c>
       <c r="D39" s="1"/>
@@ -8768,7 +8754,7 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="28">
         <v>1</v>
@@ -8788,14 +8774,14 @@
       <c r="M39" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N39" s="18">
+      <c r="N39" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="18">
         <v>500</v>
@@ -8807,7 +8793,7 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H40" s="28">
         <v>1</v>
@@ -8832,9 +8818,9 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="18">
         <v>500</v>
@@ -8846,7 +8832,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H41" s="28">
         <v>1</v>
@@ -8871,21 +8857,21 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="18">
         <v>500</v>
       </c>
-      <c r="D42" s="18"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="18">
-        <f t="shared" ref="E42:E48" si="4">LN(C42)/(C42)</f>
+        <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="F42" s="18"/>
+      <c r="F42" s="1"/>
       <c r="G42" s="18">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H42" s="28">
         <v>1</v>
@@ -8909,54 +8895,51 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="47"/>
+      <c r="B43" s="19">
+        <v>5</v>
+      </c>
+      <c r="C43" s="18">
+        <v>500</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18">
+        <f t="shared" ref="E43:E49" si="4">LN(C43)/(C43)</f>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18">
+        <v>100</v>
+      </c>
+      <c r="H43" s="28">
+        <v>1</v>
+      </c>
+      <c r="I43" s="18">
+        <v>100</v>
+      </c>
+      <c r="J43" s="18">
+        <v>1</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B44" s="23">
         <v>1</v>
-      </c>
-      <c r="C43" s="20">
-        <v>100</v>
-      </c>
-      <c r="D43" s="20">
-        <f>2*LOG(C43)/(C43-1)</f>
-        <v>4.0404040404040407E-2</v>
-      </c>
-      <c r="E43" s="20">
-        <f t="shared" si="4"/>
-        <v>4.6051701859880917E-2</v>
-      </c>
-      <c r="F43" s="20">
-        <v>4.7E-2</v>
-      </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20">
-        <v>1</v>
-      </c>
-      <c r="I43" s="20">
-        <v>100</v>
-      </c>
-      <c r="J43" s="20">
-        <v>1</v>
-      </c>
-      <c r="K43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="L43" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="M43" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="N43" s="20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45"/>
-      <c r="B44" s="23">
-        <v>2</v>
       </c>
       <c r="C44" s="20">
         <v>100</v>
@@ -8974,7 +8957,7 @@
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="20">
         <v>100</v>
@@ -8991,20 +8974,20 @@
       <c r="M44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N44" s="22">
+      <c r="N44" s="20">
         <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="20">
         <v>100</v>
       </c>
       <c r="D45" s="20">
-        <f t="shared" ref="D45:D47" si="5">2*LOG(C45)/(C45-1)</f>
+        <f>2*LOG(C45)/(C45-1)</f>
         <v>4.0404040404040407E-2</v>
       </c>
       <c r="E45" s="20">
@@ -9016,7 +8999,7 @@
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I45" s="20">
         <v>100</v>
@@ -9038,15 +9021,15 @@
       </c>
     </row>
     <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="20">
         <v>100</v>
       </c>
       <c r="D46" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D46:D48" si="5">2*LOG(C46)/(C46-1)</f>
         <v>4.0404040404040407E-2</v>
       </c>
       <c r="E46" s="20">
@@ -9058,7 +9041,7 @@
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I46" s="20">
         <v>100</v>
@@ -9080,41 +9063,41 @@
       </c>
     </row>
     <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="23">
-        <v>5</v>
-      </c>
-      <c r="C47" s="22">
+        <v>4</v>
+      </c>
+      <c r="C47" s="20">
         <v>100</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="20">
         <f t="shared" si="5"/>
         <v>4.0404040404040407E-2</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="20">
         <f t="shared" si="4"/>
         <v>4.6051701859880917E-2</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="20">
         <v>4.7E-2</v>
       </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22">
-        <v>16</v>
-      </c>
-      <c r="I47" s="22">
+      <c r="G47" s="20"/>
+      <c r="H47" s="20">
+        <v>8</v>
+      </c>
+      <c r="I47" s="20">
         <v>100</v>
       </c>
-      <c r="J47" s="22">
+      <c r="J47" s="20">
         <v>1</v>
       </c>
-      <c r="K47" s="22" t="s">
+      <c r="K47" s="20" t="s">
         <v>8</v>
       </c>
       <c r="L47" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="M47" s="22" t="s">
+      <c r="M47" s="20" t="s">
         <v>10</v>
       </c>
       <c r="N47" s="22">
@@ -9122,14 +9105,17 @@
       </c>
     </row>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="45"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="22">
         <v>100</v>
       </c>
-      <c r="D48" s="22"/>
+      <c r="D48" s="22">
+        <f t="shared" si="5"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
       <c r="E48" s="22">
         <f t="shared" si="4"/>
         <v>4.6051701859880917E-2</v>
@@ -9139,7 +9125,7 @@
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="22">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I48" s="22">
         <v>100</v>
@@ -9160,36 +9146,75 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="47"/>
+      <c r="B49" s="23">
+        <v>6</v>
+      </c>
+      <c r="C49" s="22">
+        <v>100</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22">
+        <f t="shared" si="4"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F49" s="22">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22">
+        <v>32</v>
+      </c>
+      <c r="I49" s="22">
+        <v>100</v>
+      </c>
+      <c r="J49" s="22">
+        <v>1</v>
+      </c>
+      <c r="K49" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L49" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M49" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9200,8 +9225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB93F79-F640-47DC-B202-CD46132620C4}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9242,6 +9267,9 @@
       <c r="H1" s="5">
         <v>7</v>
       </c>
+      <c r="I1" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="40">
@@ -9262,6 +9290,9 @@
       <c r="G2" s="39">
         <v>303.96879702199197</v>
       </c>
+      <c r="H2" s="46">
+        <v>101.618453169739</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="40">
@@ -9282,6 +9313,9 @@
       <c r="G3" s="39">
         <v>317.33205455264999</v>
       </c>
+      <c r="H3" s="46">
+        <v>16.106386733265001</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="40">
@@ -9302,6 +9336,9 @@
       <c r="G4" s="39">
         <v>98.939995244922997</v>
       </c>
+      <c r="H4" s="46">
+        <v>267.10079454760597</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="40">
@@ -9322,6 +9359,9 @@
       <c r="G5" s="39">
         <v>55.390225773659999</v>
       </c>
+      <c r="H5" s="46">
+        <v>686.79879814043295</v>
+      </c>
       <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -9343,6 +9383,9 @@
       <c r="G6" s="39">
         <v>4.1771041653900003</v>
       </c>
+      <c r="H6" s="46">
+        <v>784.42556102720198</v>
+      </c>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -9364,6 +9407,9 @@
       <c r="G7" s="39">
         <v>80.111976598406002</v>
       </c>
+      <c r="H7" s="46">
+        <v>592.38447247795398</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="40">
@@ -9384,6 +9430,7 @@
       <c r="G8" s="39">
         <v>40.653356154584998</v>
       </c>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="40">
@@ -9684,15 +9731,15 @@
       <c r="G23" s="39">
         <v>273.919915629147</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="40">
@@ -9716,18 +9763,18 @@
       <c r="J24" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49" t="s">
+      <c r="L24" s="52"/>
+      <c r="M24" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49" t="s">
+      <c r="N24" s="52"/>
+      <c r="O24" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="P24" s="49"/>
+      <c r="P24" s="52"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="40">
@@ -9754,18 +9801,18 @@
       <c r="J25" s="37">
         <v>10</v>
       </c>
-      <c r="K25" s="49">
+      <c r="K25" s="52">
         <v>1.2</v>
       </c>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49">
+      <c r="L25" s="52"/>
+      <c r="M25" s="52">
         <v>3</v>
       </c>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49">
+      <c r="N25" s="52"/>
+      <c r="O25" s="52">
         <v>1.7929999999999999</v>
       </c>
-      <c r="P25" s="49"/>
+      <c r="P25" s="52"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="40">
@@ -9792,18 +9839,18 @@
       <c r="J26" s="37">
         <v>20</v>
       </c>
-      <c r="K26" s="49">
+      <c r="K26" s="52">
         <v>1.3</v>
       </c>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49">
+      <c r="L26" s="52"/>
+      <c r="M26" s="52">
         <v>4</v>
       </c>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49">
+      <c r="N26" s="52"/>
+      <c r="O26" s="52">
         <v>1.8839999999999999</v>
       </c>
-      <c r="P26" s="49"/>
+      <c r="P26" s="52"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="40">
@@ -9830,18 +9877,18 @@
       <c r="J27" s="37">
         <v>50</v>
       </c>
-      <c r="K27" s="49">
+      <c r="K27" s="52">
         <v>2.36</v>
       </c>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49">
+      <c r="L27" s="52"/>
+      <c r="M27" s="52">
         <v>6</v>
       </c>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49">
+      <c r="N27" s="52"/>
+      <c r="O27" s="52">
         <v>2.2669999999999999</v>
       </c>
-      <c r="P27" s="49"/>
+      <c r="P27" s="52"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="40">
@@ -9868,18 +9915,18 @@
       <c r="J28" s="37">
         <v>100</v>
       </c>
-      <c r="K28" s="49">
+      <c r="K28" s="52">
         <v>2.5499999999999998</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49">
+      <c r="L28" s="52"/>
+      <c r="M28" s="52">
         <v>8</v>
       </c>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49">
+      <c r="N28" s="52"/>
+      <c r="O28" s="52">
         <v>2.8820000000000001</v>
       </c>
-      <c r="P28" s="49"/>
+      <c r="P28" s="52"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="40">
@@ -9906,12 +9953,12 @@
       <c r="J29" s="37">
         <v>500</v>
       </c>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="40">
@@ -9938,18 +9985,18 @@
       <c r="J30" s="37">
         <v>1000</v>
       </c>
-      <c r="K30" s="49">
+      <c r="K30" s="52">
         <v>3.55</v>
       </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49">
+      <c r="L30" s="52"/>
+      <c r="M30" s="52">
         <v>12</v>
       </c>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49">
+      <c r="N30" s="52"/>
+      <c r="O30" s="52">
         <v>4.1079999999999997</v>
       </c>
-      <c r="P30" s="49"/>
+      <c r="P30" s="52"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="40">
@@ -11271,7 +11318,7 @@
         <v>81.751524956287</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B97" s="40">
         <v>0.50833333333499997</v>
       </c>
@@ -11291,7 +11338,7 @@
         <v>240.04494272865</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B98" s="40">
         <v>8.1273675617759995</v>
       </c>
@@ -11311,7 +11358,7 @@
         <v>101.786364776827</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B99" s="40">
         <v>0.406666666668</v>
       </c>
@@ -11331,7 +11378,7 @@
         <v>134.05761535420999</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B100" s="40">
         <v>0.406666666668</v>
       </c>
@@ -11351,7 +11398,7 @@
         <v>135.39656674438999</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B101" s="40">
         <v>0.50833333333499997</v>
       </c>
@@ -11371,7 +11418,7 @@
         <v>153.03032980178801</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B102" s="42"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -11379,7 +11426,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B103" s="44">
         <v>4.5390360000000003</v>
       </c>
@@ -11398,8 +11445,11 @@
       <c r="G103" s="44">
         <v>190.18340000000001</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H103" s="46">
+        <v>408.07240000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B104" s="43">
         <v>7.9502920000000001</v>
       </c>
@@ -11418,8 +11468,11 @@
       <c r="G104" s="39">
         <v>136.82740000000001</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H104" s="46">
+        <v>322.71519999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B105" s="43">
         <v>1.5582290000000001</v>
       </c>
@@ -11438,8 +11491,11 @@
       <c r="G105" s="39">
         <v>26.817689999999999</v>
       </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H105" s="46">
+        <v>63.251010000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B106" s="43">
         <v>22</v>
       </c>
@@ -11458,8 +11514,11 @@
       <c r="G106" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H106" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B107" s="43">
         <v>78</v>
       </c>
@@ -11478,22 +11537,12 @@
       <c r="G107" s="39">
         <v>99</v>
       </c>
+      <c r="H107" s="46">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="O30:P30"/>
@@ -11503,6 +11552,19 @@
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="O29:P29"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11599,12 +11661,12 @@
       <c r="E5" s="27">
         <v>142.342376906608</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="27">
@@ -35211,19 +35273,19 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="51"/>
+      <c r="A108" s="53"/>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="51"/>
+      <c r="A109" s="53"/>
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="51"/>
+      <c r="A110" s="53"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="51"/>
+      <c r="A111" s="53"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="51"/>
+      <c r="A112" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>